<commit_message>
Delete Raw data/Montero et al., 2021/Segment points - dendrites (from Neurolucida Explorer)/SNc (mouse) directory
</commit_message>
<xml_diff>
--- a/Data analysis/VTA morphology data.xlsx
+++ b/Data analysis/VTA morphology data.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\MATLAB\Neuroanatomia\Github (scripts finales)\v1\Raw data\Montero et al., 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rigat\Documents\GitHub\Neuronal-Convex-hull-intersection\Data analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99171034-AA0F-483F-8F4B-6BA449DEF697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEE1E04-5CF7-407A-A899-8599FD68FB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{997D98C6-60AC-48FA-BAF3-9348660132A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Morphology" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -132,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,11 +195,6 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -411,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -438,26 +432,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -466,7 +447,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,20 +456,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,31 +500,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,7 +833,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,26 +847,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="31" t="s">
         <v>23</v>
       </c>
@@ -892,7 +885,7 @@
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
       <c r="R2" s="33"/>
-      <c r="S2" s="38" t="s">
+      <c r="S2" s="34" t="s">
         <v>25</v>
       </c>
       <c r="T2" s="32"/>
@@ -900,7 +893,7 @@
       <c r="V2" s="33"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -913,1012 +906,1012 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="40" t="s">
+      <c r="Q3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="41" t="s">
+      <c r="R3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="40" t="s">
+      <c r="T3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="40" t="s">
+      <c r="U3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="41" t="s">
+      <c r="V3" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="12">
         <v>6076.1</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="12">
         <v>5</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="12">
         <v>36</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="13">
         <v>3.8909271000000002E-2</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="24">
         <v>28.263480900000001</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="12">
         <v>0.50023859999999998</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="12">
         <v>22.9714831</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="13">
         <v>2.6805548699999999</v>
       </c>
-      <c r="K4" s="34">
+      <c r="K4" s="24">
         <v>17.949350800000001</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="12">
         <v>7.2649783599999997</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="12">
         <v>16.919254200000001</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="13">
         <v>3.4506590300000002</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="24">
         <v>16.668397850127601</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="12">
         <v>0.53594419092384904</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="12">
         <v>30.147247317264998</v>
       </c>
-      <c r="R4" s="20">
+      <c r="R4" s="13">
         <v>11.6388543059018</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="12">
         <v>14.3218003366198</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="12">
         <v>1.09820943630433</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U4" s="12">
         <v>21.6097435292026</v>
       </c>
-      <c r="V4" s="20">
+      <c r="V4" s="13">
         <v>3.9628328894561302</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="15">
         <v>6102.1</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="15">
         <v>9</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="15">
         <v>72</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="16">
         <v>7.4088234000000003E-2</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="25">
         <v>26.0710096</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="15">
         <v>4.75327799</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="15">
         <v>27.958362399999999</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="16">
         <v>6.2114844900000001</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="25">
         <v>16.9356875</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="15">
         <v>8.0988372999999996</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="15">
         <v>9.1501715099999998</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="16">
         <v>0.82116924000000002</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="25">
         <v>13.766818375249001</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="15">
         <v>8.1850020438986402</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="15">
         <v>16.1733333960976</v>
       </c>
-      <c r="R5" s="23">
+      <c r="R5" s="16">
         <v>4.4224384990161596</v>
       </c>
-      <c r="S5" s="22">
+      <c r="S5" s="15">
         <v>20.284781850809399</v>
       </c>
-      <c r="T5" s="22">
+      <c r="T5" s="15">
         <v>10.182448934739901</v>
       </c>
-      <c r="U5" s="22">
+      <c r="U5" s="15">
         <v>20.509335483308199</v>
       </c>
-      <c r="V5" s="23">
+      <c r="V5" s="16">
         <v>6.46484428274929</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="12">
         <v>2507.5</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="12">
         <v>5</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="12">
         <v>31</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="13">
         <v>9.7140079999999997E-3</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="24">
         <v>18.9208815</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="12">
         <v>6.3127486299999997</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="12">
         <v>14.914440900000001</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="13">
         <v>0</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="24">
         <v>16.642987900000001</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="12">
         <v>9.6467133900000004</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="12">
         <v>16.4267222</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="13">
         <v>17.135505500000001</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="24">
         <v>4.8685902820462097</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="12">
         <v>2.12190711764352</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="12">
         <v>7.96236753454082</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="13">
         <v>2.1975096616181302</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="12">
         <v>18.885990877370499</v>
       </c>
-      <c r="T6" s="19">
+      <c r="T6" s="12">
         <v>21.816993237953501</v>
       </c>
-      <c r="U6" s="19">
+      <c r="U6" s="12">
         <v>31.362822780842301</v>
       </c>
-      <c r="V6" s="20">
+      <c r="V6" s="13">
         <v>10.7598767853328</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4">
         <v>7</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="15">
         <v>6330.1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="15">
         <v>5</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="15">
         <v>34</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="16">
         <v>6.8728335000000002E-2</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="25">
         <v>0.43975176999999999</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="15">
         <v>2.0558953500000001</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="15">
         <v>8.1432206800000007</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="16">
         <v>0</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="25">
         <v>53.3617572</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="15">
         <v>4.5716326599999997</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="15">
         <v>31.427742299999998</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="16">
         <v>0</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="25">
         <v>1.60304046876415</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="15">
         <v>2.4896883826909302</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="15">
         <v>11.590912084875299</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="16">
         <v>2.5609564506571401</v>
       </c>
-      <c r="S7" s="22">
+      <c r="S7" s="15">
         <v>10.221099380761199</v>
       </c>
-      <c r="T7" s="22">
+      <c r="T7" s="15">
         <v>0.36896919362546099</v>
       </c>
-      <c r="U7" s="22">
+      <c r="U7" s="15">
         <v>18.761008096329501</v>
       </c>
-      <c r="V7" s="23">
+      <c r="V7" s="16">
         <v>52.382203007425403</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="12">
         <v>4475.8</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="12">
         <v>9</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="12">
         <v>41</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="13">
         <v>1.3596064999999999E-2</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="24">
         <v>15.741163999999999</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="12">
         <v>5.135459</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="12">
         <v>16.460152900000001</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="13">
         <v>0.40396802999999998</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="24">
         <v>29.256180000000001</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="12">
         <v>2.0606075599999998</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="12">
         <v>27.5871867</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="13">
         <v>3.3552818499999999</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="24">
         <v>9.60720432693841</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="12">
         <v>3.2109756892968502</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="12">
         <v>10.561487220986301</v>
       </c>
-      <c r="R8" s="20">
+      <c r="R8" s="13">
         <v>1.0845765591498</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="12">
         <v>22.406033462683599</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="12">
         <v>9.7477557496279399</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="12">
         <v>23.772041397073099</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="13">
         <v>19.593734294294499</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="15">
         <v>5406.4</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="15">
         <v>5</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="15">
         <v>29</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="16">
         <v>4.9140126999999999E-2</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="25">
         <v>23.895579399999999</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="15">
         <v>0</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="15">
         <v>18.702151499999999</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="16">
         <v>19.287592400000001</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="25">
         <v>4.19106004</v>
       </c>
-      <c r="L9" s="22">
+      <c r="L9" s="15">
         <v>1.6342955100000001</v>
       </c>
-      <c r="M9" s="22">
+      <c r="M9" s="15">
         <v>22.984732000000001</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="16">
         <v>9.3045890999999994</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="25">
         <v>1.9317181883588801</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="15">
         <v>0.55664687913138</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="15">
         <v>11.214358742588001</v>
       </c>
-      <c r="R9" s="23">
+      <c r="R9" s="16">
         <v>0.41799974704959503</v>
       </c>
-      <c r="S9" s="22">
+      <c r="S9" s="15">
         <v>22.0619070812308</v>
       </c>
-      <c r="T9" s="22">
+      <c r="T9" s="15">
         <v>7.1734330412659597</v>
       </c>
-      <c r="U9" s="22">
+      <c r="U9" s="15">
         <v>55.572294462323597</v>
       </c>
-      <c r="V9" s="23">
+      <c r="V9" s="16">
         <v>1.02065495142706</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="12">
         <v>3322.5</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="12">
         <v>3</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="12">
         <v>19</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="13">
         <v>1.9931962000000001E-2</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="24">
         <v>26.488539299999999</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="12">
         <v>0.16049550000000001</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="12">
         <v>25.810389300000001</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="13">
         <v>1.67955152</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="24">
         <v>10.481938599999999</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="12">
         <v>0</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="12">
         <v>28.595325299999999</v>
       </c>
-      <c r="N10" s="20">
+      <c r="N10" s="13">
         <v>6.7837605700000001</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="24">
         <v>11.7723263739143</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="12">
         <v>0.40357138458855302</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="12">
         <v>11.6286688960856</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="13">
         <v>37.527050563830102</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="12">
         <v>3.9805931928231999</v>
       </c>
-      <c r="T10" s="19">
+      <c r="T10" s="12">
         <v>1.09748079103834</v>
       </c>
-      <c r="U10" s="19">
+      <c r="U10" s="12">
         <v>20.941606715635402</v>
       </c>
-      <c r="V10" s="20">
+      <c r="V10" s="13">
         <v>12.6365532362345</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="4">
         <v>6</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <v>8093.5</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="15">
         <v>9</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="15">
         <v>74</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="16">
         <v>6.3295614E-2</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="25">
         <v>9.0632080599999991</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="15">
         <v>2.7970935200000002</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="15">
         <v>7.16071568</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="16">
         <v>3.7561528200000001</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="25">
         <v>35.168763200000001</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="15">
         <v>4.37534182</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="15">
         <v>37.678724899999999</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="16">
         <v>0</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="25">
         <v>1.0329990129259301</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="15">
         <v>5.4199468620432496</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="15">
         <v>1.06160336291403</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="16">
         <v>8.6665573001052404E-2</v>
       </c>
-      <c r="S11" s="22">
+      <c r="S11" s="15">
         <v>33.819309615307901</v>
       </c>
-      <c r="T11" s="22">
+      <c r="T11" s="15">
         <v>10.5423087023748</v>
       </c>
-      <c r="U11" s="22">
+      <c r="U11" s="15">
         <v>27.594006430658499</v>
       </c>
-      <c r="V11" s="23">
+      <c r="V11" s="16">
         <v>20.426097146347001</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3">
         <v>6</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="12">
         <v>6880.5</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="12">
         <v>7</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="12">
         <v>41</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="13">
         <v>0.10185366699999999</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="24">
         <v>11.947202600000001</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="12">
         <v>0.78159268999999998</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="12">
         <v>14.5551701</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="13">
         <v>0.27515253000000001</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="24">
         <v>25.577222200000001</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="12">
         <v>14.78247</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="12">
         <v>32.081189899999998</v>
       </c>
-      <c r="N12" s="20">
+      <c r="N12" s="13">
         <v>0</v>
       </c>
-      <c r="O12" s="34">
+      <c r="O12" s="24">
         <v>6.7001826297614704</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="12">
         <v>2.2294227643351201</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="12">
         <v>13.618887684397</v>
       </c>
-      <c r="R12" s="20">
+      <c r="R12" s="13">
         <v>0.82934682305799601</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="12">
         <v>26.465454109428698</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="12">
         <v>10.167063850462201</v>
       </c>
-      <c r="U12" s="19">
+      <c r="U12" s="12">
         <v>38.175470678778403</v>
       </c>
-      <c r="V12" s="20">
+      <c r="V12" s="13">
         <v>1.79979260674956</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="4">
         <v>6</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="15">
         <v>4423.7</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="15">
         <v>7</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="15">
         <v>27</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="16">
         <v>5.6206809000000003E-2</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="25">
         <v>3.2644487299999998</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="15">
         <v>11.266606100000001</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="15">
         <v>7.3634608799999999</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="16">
         <v>0.16748041</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="25">
         <v>17.443510799999999</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="15">
         <v>0</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="15">
         <v>20.866924000000001</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="16">
         <v>39.627569000000001</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="25">
         <v>6.4286474122543904</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="15">
         <v>4.3418737599240398</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="15">
         <v>31.3707752027642</v>
       </c>
-      <c r="R13" s="23">
+      <c r="R13" s="16">
         <v>10.3516236041882</v>
       </c>
-      <c r="S13" s="22">
+      <c r="S13" s="15">
         <v>2.5932848353750599</v>
       </c>
-      <c r="T13" s="22">
+      <c r="T13" s="15">
         <v>1.9737496644451999</v>
       </c>
-      <c r="U13" s="22">
+      <c r="U13" s="15">
         <v>27.7625087736794</v>
       </c>
-      <c r="V13" s="23">
+      <c r="V13" s="16">
         <v>15.1693155949689</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="12">
         <v>5118.2</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="12">
         <v>7</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="12">
         <v>35</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="13">
         <v>5.9278800999999999E-2</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="24">
         <v>11.791135799999999</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="12">
         <v>0</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="12">
         <v>9.1359576899999997</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="13">
         <v>36.815635200000003</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K14" s="24">
         <v>12.4493834</v>
       </c>
-      <c r="L14" s="19">
+      <c r="L14" s="12">
         <v>0.35500988999999999</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="12">
         <v>22.417395500000001</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="13">
         <v>7.0354824999999996</v>
       </c>
-      <c r="O14" s="34">
+      <c r="O14" s="24">
         <v>8.5926049257926298</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="12">
         <v>2.9772675849602601</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="Q14" s="12">
         <v>25.296858203016701</v>
       </c>
-      <c r="R14" s="20">
+      <c r="R14" s="13">
         <v>8.8602946797883195</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="12">
         <v>7.8300121214386298</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="12">
         <v>0.87386534244122205</v>
       </c>
-      <c r="U14" s="19">
+      <c r="U14" s="12">
         <v>36.119166652583601</v>
       </c>
-      <c r="V14" s="20">
+      <c r="V14" s="13">
         <v>9.4375559466207601</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="4">
         <v>5</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="15">
         <v>3989</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="15">
         <v>4</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="15">
         <v>15</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="16">
         <v>5.5108156999999998E-2</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="25">
         <v>4.5134500000000001E-2</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="15">
         <v>12.7429741</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="15">
         <v>9.1532767600000007</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="16">
         <v>0</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="25">
         <v>24.174038599999999</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="15">
         <v>7.9767707799999998</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="15">
         <v>24.754769199999998</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="16">
         <v>21.153036</v>
       </c>
-      <c r="O15" s="35">
+      <c r="O15" s="25">
         <v>6.2529056738692903</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="15">
         <v>6.7400274345922204</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="15">
         <v>5.8409363400244603</v>
       </c>
-      <c r="R15" s="23">
+      <c r="R15" s="16">
         <v>1.95412535723773</v>
       </c>
-      <c r="S15" s="22">
+      <c r="S15" s="15">
         <v>26.797196843916499</v>
       </c>
-      <c r="T15" s="22">
+      <c r="T15" s="15">
         <v>29.574668150415199</v>
       </c>
-      <c r="U15" s="22">
+      <c r="U15" s="15">
         <v>21.417526154907499</v>
       </c>
-      <c r="V15" s="23">
+      <c r="V15" s="16">
         <v>1.4097934244538499</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="5">
         <v>5</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="18">
         <v>3522.7</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="18">
         <v>4</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="18">
         <v>21</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="19">
         <v>2.3360961E-2</v>
       </c>
-      <c r="G16" s="36">
+      <c r="G16" s="26">
         <v>27.112949700000001</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="18">
         <v>17.021436600000001</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="18">
         <v>11.7262129</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="19">
         <v>0</v>
       </c>
-      <c r="K16" s="36">
+      <c r="K16" s="26">
         <v>19.764322400000001</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="18">
         <v>12.54607</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="18">
         <v>11.829008399999999</v>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="19">
         <v>0</v>
       </c>
-      <c r="O16" s="36">
+      <c r="O16" s="26">
         <v>41.958507331512401</v>
       </c>
-      <c r="P16" s="25">
+      <c r="P16" s="18">
         <v>32.3499920168559</v>
       </c>
-      <c r="Q16" s="25">
+      <c r="Q16" s="18">
         <v>2.6957503246725101</v>
       </c>
-      <c r="R16" s="26">
+      <c r="R16" s="19">
         <v>0.48272588873348299</v>
       </c>
-      <c r="S16" s="25">
+      <c r="S16" s="18">
         <v>9.8887617897092106</v>
       </c>
-      <c r="T16" s="25">
+      <c r="T16" s="18">
         <v>9.6615278104603597</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="18">
         <v>2.81938687082779</v>
       </c>
-      <c r="V16" s="26">
+      <c r="V16" s="19">
         <v>0.129838852261282</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="21">
         <v>4349.3</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="21">
         <v>5</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="21">
         <v>28</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="16">
         <v>4.7811899999999997E-2</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="25">
         <v>21.502310699999999</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="15">
         <v>0</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="15">
         <v>8.2955877999999998</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="16">
         <v>17.5085646</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="25">
         <v>12.7744695</v>
       </c>
-      <c r="L17" s="22">
+      <c r="L17" s="15">
         <v>1.42091831</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="15">
         <v>38.498149099999999</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="16">
         <v>0</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="25">
         <v>10.937378558879599</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="15">
         <v>0.286884744617601</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="15">
         <v>4.9633236596274202</v>
       </c>
-      <c r="R17" s="23">
+      <c r="R17" s="16">
         <v>14.2538161780235</v>
       </c>
-      <c r="S17" s="22">
+      <c r="S17" s="15">
         <v>23.807960909651499</v>
       </c>
-      <c r="T17" s="22">
+      <c r="T17" s="15">
         <v>3.6987095614886201</v>
       </c>
-      <c r="U17" s="22">
+      <c r="U17" s="15">
         <v>33.332839426420499</v>
       </c>
-      <c r="V17" s="23">
+      <c r="V17" s="16">
         <v>8.7041845709190895</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="7">
@@ -1933,10 +1926,10 @@
       <c r="E18" s="9">
         <v>43</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="23">
         <v>5.3962000000000003E-2</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="27">
         <v>33.561361400000003</v>
       </c>
       <c r="H18" s="9">
@@ -1945,10 +1938,10 @@
       <c r="I18" s="9">
         <v>12.8814004</v>
       </c>
-      <c r="J18" s="30">
+      <c r="J18" s="23">
         <v>10.148811800000001</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="27">
         <v>31.531599100000001</v>
       </c>
       <c r="L18" s="9">
@@ -1957,10 +1950,10 @@
       <c r="M18" s="9">
         <v>0</v>
       </c>
-      <c r="N18" s="30">
+      <c r="N18" s="23">
         <v>0.48354448999999999</v>
       </c>
-      <c r="O18" s="37">
+      <c r="O18" s="27">
         <v>44.751094548619598</v>
       </c>
       <c r="P18" s="9">
@@ -1969,7 +1962,7 @@
       <c r="Q18" s="9">
         <v>3.4212517168524599</v>
       </c>
-      <c r="R18" s="30">
+      <c r="R18" s="23">
         <v>12.010046781137</v>
       </c>
       <c r="S18" s="9">
@@ -1981,7 +1974,7 @@
       <c r="U18" s="9">
         <v>0.49871181972188899</v>
       </c>
-      <c r="V18" s="30">
+      <c r="V18" s="23">
         <v>0.44871391194615901</v>
       </c>
     </row>
@@ -1999,643 +1992,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FB300B-6797-4DB8-8B18-DB79091E014B}">
-  <dimension ref="B3:W30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:I22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="42">
-        <v>14.3218003366198</v>
-      </c>
-      <c r="C3" s="42">
-        <v>20.284781850809399</v>
-      </c>
-      <c r="D3" s="42">
-        <v>18.885990877370499</v>
-      </c>
-      <c r="E3" s="42">
-        <v>10.221099380761199</v>
-      </c>
-      <c r="F3" s="42">
-        <v>22.406033462683599</v>
-      </c>
-      <c r="G3" s="42">
-        <v>22.0619070812308</v>
-      </c>
-      <c r="H3" s="42">
-        <v>3.9805931928231999</v>
-      </c>
-      <c r="I3" s="42">
-        <v>33.819309615307901</v>
-      </c>
-      <c r="J3" s="42">
-        <v>26.465454109428698</v>
-      </c>
-      <c r="K3" s="42">
-        <v>2.5932848353750599</v>
-      </c>
-      <c r="L3" s="42">
-        <v>7.8300121214386298</v>
-      </c>
-      <c r="M3" s="42">
-        <v>26.797196843916499</v>
-      </c>
-      <c r="N3" s="42">
-        <v>9.8887617897092106</v>
-      </c>
-      <c r="O3" s="42">
-        <v>23.807960909651499</v>
-      </c>
-      <c r="P3" s="42">
-        <v>29.663637988207601</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="42">
-        <v>1.09820943630433</v>
-      </c>
-      <c r="C4" s="42">
-        <v>10.182448934739901</v>
-      </c>
-      <c r="D4" s="42">
-        <v>21.816993237953501</v>
-      </c>
-      <c r="E4" s="42">
-        <v>0.36896919362546099</v>
-      </c>
-      <c r="F4" s="42">
-        <v>9.7477557496279399</v>
-      </c>
-      <c r="G4" s="42">
-        <v>7.1734330412659597</v>
-      </c>
-      <c r="H4" s="42">
-        <v>1.09748079103834</v>
-      </c>
-      <c r="I4" s="42">
-        <v>10.5423087023748</v>
-      </c>
-      <c r="J4" s="42">
-        <v>10.167063850462201</v>
-      </c>
-      <c r="K4" s="42">
-        <v>1.9737496644451999</v>
-      </c>
-      <c r="L4" s="42">
-        <v>0.87386534244122205</v>
-      </c>
-      <c r="M4" s="42">
-        <v>29.574668150415199</v>
-      </c>
-      <c r="N4" s="42">
-        <v>9.6615278104603597</v>
-      </c>
-      <c r="O4" s="42">
-        <v>3.6987095614886201</v>
-      </c>
-      <c r="P4" s="42">
-        <v>4.8784481145716603</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="42">
-        <v>21.6097435292026</v>
-      </c>
-      <c r="C5" s="42">
-        <v>20.509335483308199</v>
-      </c>
-      <c r="D5" s="42">
-        <v>31.362822780842301</v>
-      </c>
-      <c r="E5" s="42">
-        <v>18.761008096329501</v>
-      </c>
-      <c r="F5" s="42">
-        <v>23.772041397073099</v>
-      </c>
-      <c r="G5" s="42">
-        <v>55.572294462323597</v>
-      </c>
-      <c r="H5" s="42">
-        <v>20.941606715635402</v>
-      </c>
-      <c r="I5" s="42">
-        <v>27.594006430658499</v>
-      </c>
-      <c r="J5" s="42">
-        <v>38.175470678778403</v>
-      </c>
-      <c r="K5" s="42">
-        <v>27.7625087736794</v>
-      </c>
-      <c r="L5" s="42">
-        <v>36.119166652583601</v>
-      </c>
-      <c r="M5" s="42">
-        <v>21.417526154907499</v>
-      </c>
-      <c r="N5" s="42">
-        <v>2.81938687082779</v>
-      </c>
-      <c r="O5" s="42">
-        <v>33.332839426420499</v>
-      </c>
-      <c r="P5" s="42">
-        <v>0.49871181972188899</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="42">
-        <v>3.9628328894561302</v>
-      </c>
-      <c r="C6" s="42">
-        <v>6.46484428274929</v>
-      </c>
-      <c r="D6" s="42">
-        <v>10.7598767853328</v>
-      </c>
-      <c r="E6" s="42">
-        <v>52.382203007425403</v>
-      </c>
-      <c r="F6" s="42">
-        <v>19.593734294294499</v>
-      </c>
-      <c r="G6" s="42">
-        <v>1.02065495142706</v>
-      </c>
-      <c r="H6" s="42">
-        <v>12.6365532362345</v>
-      </c>
-      <c r="I6" s="42">
-        <v>20.426097146347001</v>
-      </c>
-      <c r="J6" s="42">
-        <v>1.79979260674956</v>
-      </c>
-      <c r="K6" s="42">
-        <v>15.1693155949689</v>
-      </c>
-      <c r="L6" s="42">
-        <v>9.4375559466207601</v>
-      </c>
-      <c r="M6" s="42">
-        <v>1.4097934244538499</v>
-      </c>
-      <c r="N6" s="42">
-        <v>0.129838852261282</v>
-      </c>
-      <c r="O6" s="42">
-        <v>8.7041845709190895</v>
-      </c>
-      <c r="P6" s="42">
-        <v>0.44871391194615901</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="F8" s="42">
-        <v>14.3218003366198</v>
-      </c>
-      <c r="G8" s="42">
-        <v>1.09820943630433</v>
-      </c>
-      <c r="H8" s="42">
-        <v>21.6097435292026</v>
-      </c>
-      <c r="I8" s="42">
-        <v>3.9628328894561302</v>
-      </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="F9" s="42">
-        <v>20.284781850809399</v>
-      </c>
-      <c r="G9" s="42">
-        <v>10.182448934739901</v>
-      </c>
-      <c r="H9" s="42">
-        <v>20.509335483308199</v>
-      </c>
-      <c r="I9" s="42">
-        <v>6.46484428274929</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42">
-        <v>18.885990877370499</v>
-      </c>
-      <c r="G10" s="42">
-        <v>21.816993237953501</v>
-      </c>
-      <c r="H10" s="42">
-        <v>31.362822780842301</v>
-      </c>
-      <c r="I10" s="42">
-        <v>10.7598767853328</v>
-      </c>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="42"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42">
-        <v>10.221099380761199</v>
-      </c>
-      <c r="G11" s="42">
-        <v>0.36896919362546099</v>
-      </c>
-      <c r="H11" s="42">
-        <v>18.761008096329501</v>
-      </c>
-      <c r="I11" s="42">
-        <v>52.382203007425403</v>
-      </c>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42">
-        <v>22.406033462683599</v>
-      </c>
-      <c r="G12" s="42">
-        <v>9.7477557496279399</v>
-      </c>
-      <c r="H12" s="42">
-        <v>23.772041397073099</v>
-      </c>
-      <c r="I12" s="42">
-        <v>19.593734294294499</v>
-      </c>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42">
-        <v>22.0619070812308</v>
-      </c>
-      <c r="G13" s="42">
-        <v>7.1734330412659597</v>
-      </c>
-      <c r="H13" s="42">
-        <v>55.572294462323597</v>
-      </c>
-      <c r="I13" s="42">
-        <v>1.02065495142706</v>
-      </c>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
-      <c r="U13" s="42"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42">
-        <v>3.9805931928231999</v>
-      </c>
-      <c r="G14" s="42">
-        <v>1.09748079103834</v>
-      </c>
-      <c r="H14" s="42">
-        <v>20.941606715635402</v>
-      </c>
-      <c r="I14" s="42">
-        <v>12.6365532362345</v>
-      </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42">
-        <v>33.819309615307901</v>
-      </c>
-      <c r="G15" s="42">
-        <v>10.5423087023748</v>
-      </c>
-      <c r="H15" s="42">
-        <v>27.594006430658499</v>
-      </c>
-      <c r="I15" s="42">
-        <v>20.426097146347001</v>
-      </c>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42">
-        <v>26.465454109428698</v>
-      </c>
-      <c r="G16" s="42">
-        <v>10.167063850462201</v>
-      </c>
-      <c r="H16" s="42">
-        <v>38.175470678778403</v>
-      </c>
-      <c r="I16" s="42">
-        <v>1.79979260674956</v>
-      </c>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42">
-        <v>2.5932848353750599</v>
-      </c>
-      <c r="G17" s="42">
-        <v>1.9737496644451999</v>
-      </c>
-      <c r="H17" s="42">
-        <v>27.7625087736794</v>
-      </c>
-      <c r="I17" s="42">
-        <v>15.1693155949689</v>
-      </c>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42">
-        <v>7.8300121214386298</v>
-      </c>
-      <c r="G18" s="42">
-        <v>0.87386534244122205</v>
-      </c>
-      <c r="H18" s="42">
-        <v>36.119166652583601</v>
-      </c>
-      <c r="I18" s="42">
-        <v>9.4375559466207601</v>
-      </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42">
-        <v>26.797196843916499</v>
-      </c>
-      <c r="G19" s="42">
-        <v>29.574668150415199</v>
-      </c>
-      <c r="H19" s="42">
-        <v>21.417526154907499</v>
-      </c>
-      <c r="I19" s="42">
-        <v>1.4097934244538499</v>
-      </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42">
-        <v>9.8887617897092106</v>
-      </c>
-      <c r="G20" s="42">
-        <v>9.6615278104603597</v>
-      </c>
-      <c r="H20" s="42">
-        <v>2.81938687082779</v>
-      </c>
-      <c r="I20" s="42">
-        <v>0.129838852261282</v>
-      </c>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42">
-        <v>23.807960909651499</v>
-      </c>
-      <c r="G21" s="42">
-        <v>3.6987095614886201</v>
-      </c>
-      <c r="H21" s="42">
-        <v>33.332839426420499</v>
-      </c>
-      <c r="I21" s="42">
-        <v>8.7041845709190895</v>
-      </c>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42">
-        <v>29.663637988207601</v>
-      </c>
-      <c r="G22" s="42">
-        <v>4.8784481145716603</v>
-      </c>
-      <c r="H22" s="42">
-        <v>0.49871181972188899</v>
-      </c>
-      <c r="I22" s="42">
-        <v>0.44871391194615901</v>
-      </c>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>